<commit_message>
Added options button. Choose headers and save them
</commit_message>
<xml_diff>
--- a/SecretaryST/SecretaryST.xlsx
+++ b/SecretaryST/SecretaryST.xlsx
@@ -8,19 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsi\source\repos\SecretaryST\SecretaryST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E09C318-3366-4117-B578-9040CE82F77A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CADB6F-A2DE-456D-BEA9-6B6EC76721DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20910" windowHeight="11835" tabRatio="801" xr2:uid="{4360E510-CB4A-4B4A-B617-E904287C25BF}"/>
+    <workbookView xWindow="31200" yWindow="5220" windowWidth="14670" windowHeight="8415" tabRatio="801" xr2:uid="{4360E510-CB4A-4B4A-B617-E904287C25BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="База" sheetId="3" r:id="rId1"/>
-    <sheet name="Заявка" sheetId="1" r:id="rId2"/>
+    <sheet name="OPTIONS" sheetId="4" r:id="rId1"/>
+    <sheet name="База" sheetId="3" r:id="rId2"/>
+    <sheet name="Заявка" sheetId="1" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Groups">[1]Настройка!$C$45:$C$57</definedName>
+    <definedName name="startProtAllHeaders">OPTIONS!$A$1:$D$1</definedName>
+    <definedName name="startProtHeaders1">OPTIONS!$E$1:$H$1</definedName>
+    <definedName name="startProtHeaders2">OPTIONS!$I$1:$L$1</definedName>
+    <definedName name="startProtHeaders4">OPTIONS!$M$1:$P$1</definedName>
     <definedName name="Пол">[1]Настройка!$F$116:$F$117</definedName>
     <definedName name="Разряды">[1]Настройка!$C$117:$C$128</definedName>
   </definedNames>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="66">
   <si>
     <t>№ п/п</t>
   </si>
@@ -320,6 +325,78 @@
   </si>
   <si>
     <t>Ж</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>№ П/п</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name-coop</t>
+  </si>
+  <si>
+    <t>cooperative name</t>
+  </si>
+  <si>
+    <t>Состав</t>
+  </si>
+  <si>
+    <t>person-nr</t>
+  </si>
+  <si>
+    <t>person number</t>
+  </si>
+  <si>
+    <t>Номер участника</t>
+  </si>
+  <si>
+    <t>both-nr</t>
+  </si>
+  <si>
+    <t>group-nr</t>
+  </si>
+  <si>
+    <t>rang</t>
+  </si>
+  <si>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>compeete_name</t>
+  </si>
+  <si>
+    <t>delegation</t>
+  </si>
+  <si>
+    <t>delegation-manager</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>chip_nr</t>
+  </si>
+  <si>
+    <t>distance-rang</t>
+  </si>
+  <si>
+    <t>start-time</t>
+  </si>
+  <si>
+    <t>Связка</t>
+  </si>
+  <si>
+    <t>Время старта</t>
   </si>
 </sst>
 </file>
@@ -762,6 +839,8 @@
       <sheetName val="DATA_связки"/>
       <sheetName val="DATA_группа"/>
       <sheetName val="Сводная"/>
+      <sheetName val="Старт_ЛИЧКА"/>
+      <sheetName val="Старт_ГРУППА"/>
       <sheetName val="База"/>
       <sheetName val="Тех.заявка"/>
       <sheetName val="Выписка"/>
@@ -881,6 +960,8 @@
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1182,13 +1263,263 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7BA723-EE3B-47DB-94B5-91F366626934}">
+  <sheetPr codeName="Лист2"/>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B900EF69-1E73-401A-A5D3-83A1EB74C686}">
   <sheetPr codeName="Лист3">
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:W601"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
@@ -13317,7 +13648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD62B572-980F-4A1A-87BC-FCB4965752C4}">
   <sheetPr codeName="Лист1">
     <tabColor theme="7" tint="0.59999389629810485"/>

</xml_diff>

<commit_message>
Use headers from options
</commit_message>
<xml_diff>
--- a/SecretaryST/SecretaryST.xlsx
+++ b/SecretaryST/SecretaryST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsi\source\repos\SecretaryST\SecretaryST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CADB6F-A2DE-456D-BEA9-6B6EC76721DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1749A864-DF1F-41B4-9D77-6E2512690433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="5220" windowWidth="14670" windowHeight="8415" tabRatio="801" xr2:uid="{4360E510-CB4A-4B4A-B617-E904287C25BF}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20910" windowHeight="11835" tabRatio="801" xr2:uid="{4360E510-CB4A-4B4A-B617-E904287C25BF}"/>
   </bookViews>
   <sheets>
     <sheet name="OPTIONS" sheetId="4" r:id="rId1"/>
@@ -22,10 +22,10 @@
   </externalReferences>
   <definedNames>
     <definedName name="Groups">[1]Настройка!$C$45:$C$57</definedName>
-    <definedName name="startProtAllHeaders">OPTIONS!$A$1:$D$1</definedName>
-    <definedName name="startProtHeaders1">OPTIONS!$E$1:$H$1</definedName>
-    <definedName name="startProtHeaders2">OPTIONS!$I$1:$L$1</definedName>
-    <definedName name="startProtHeaders4">OPTIONS!$M$1:$P$1</definedName>
+    <definedName name="startProtAllHeaders">OPTIONS!$A$1:$C$1</definedName>
+    <definedName name="startProtHeaders1">OPTIONS!$D$1</definedName>
+    <definedName name="startProtHeaders2">OPTIONS!$E$1</definedName>
+    <definedName name="startProtHeaders4">OPTIONS!$F$1</definedName>
     <definedName name="Пол">[1]Настройка!$F$116:$F$117</definedName>
     <definedName name="Разряды">[1]Настройка!$C$117:$C$128</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="63">
   <si>
     <t>№ п/п</t>
   </si>
@@ -330,9 +330,6 @@
     <t>nr</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>№ П/п</t>
   </si>
   <si>
@@ -342,16 +339,10 @@
     <t>name-coop</t>
   </si>
   <si>
-    <t>cooperative name</t>
-  </si>
-  <si>
     <t>Состав</t>
   </si>
   <si>
     <t>person-nr</t>
-  </si>
-  <si>
-    <t>person number</t>
   </si>
   <si>
     <t>Номер участника</t>
@@ -403,7 +394,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +402,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
@@ -550,6 +548,14 @@
       <family val="4"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -679,116 +685,121 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="19" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="16"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="18">
     <cellStyle name="Денежный 2" xfId="2" xr:uid="{208DFB5A-26C4-4A29-ACCA-1A29567B3596}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 10" xfId="17" xr:uid="{71891113-C20B-4B72-8BA2-63B31E2372FC}"/>
     <cellStyle name="Обычный 2" xfId="3" xr:uid="{11C35172-3F72-4D94-9784-0E15ABB6676E}"/>
     <cellStyle name="Обычный 2 2" xfId="4" xr:uid="{8333826C-C93A-4B0A-9AF9-4F8288911EDD}"/>
     <cellStyle name="Обычный 2 2 2" xfId="5" xr:uid="{BF2F90D4-3497-419D-98D8-9008F3102F11}"/>
@@ -802,6 +813,8 @@
     <cellStyle name="Обычный 5" xfId="13" xr:uid="{A93362C5-9EBB-41E6-8EC8-958142837B13}"/>
     <cellStyle name="Обычный 6" xfId="14" xr:uid="{24C69112-730D-4750-B171-1536D643C4FE}"/>
     <cellStyle name="Обычный 7" xfId="1" xr:uid="{B7B581BD-86E9-4F06-A676-32568A0C3507}"/>
+    <cellStyle name="Обычный 8" xfId="16" xr:uid="{DCAF0B80-53AA-4CA7-AB01-E39FAF0B9C83}"/>
+    <cellStyle name="Обычный 9" xfId="15" xr:uid="{41AB6356-57A1-4881-AE2D-4FF88F1ACC99}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1265,243 +1278,303 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7BA723-EE3B-47DB-94B5-91F366626934}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="30">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30">
+        <v>10</v>
+      </c>
+      <c r="E1" s="30">
+        <v>7</v>
+      </c>
+      <c r="F1" s="30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="30">
+        <v>3.15</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D2">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="30">
+        <v>25</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="30">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D4">
+      <c r="C5" s="30">
+        <v>10</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="30">
+        <v>10</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="30">
+        <v>10</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="30">
+        <v>7</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="30">
+        <v>5</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="30">
+        <v>5</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C11" s="30">
+        <v>14</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30">
+        <v>30</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="30">
+        <v>20</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="30">
+        <v>20</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="30">
+        <v>9</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="30">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="30">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: options sheet was not saved from deleting
</commit_message>
<xml_diff>
--- a/SecretaryST/SecretaryST.xlsx
+++ b/SecretaryST/SecretaryST.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsi\source\repos\SecretaryST\SecretaryST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1749A864-DF1F-41B4-9D77-6E2512690433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58196DF0-08AD-4D91-BE8F-43C9B045E123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20910" windowHeight="11835" tabRatio="801" xr2:uid="{4360E510-CB4A-4B4A-B617-E904287C25BF}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="20910" windowHeight="11835" tabRatio="801" firstSheet="1" activeTab="1" xr2:uid="{4360E510-CB4A-4B4A-B617-E904287C25BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="OPTIONS" sheetId="4" r:id="rId1"/>
+    <sheet name="OPTIONS" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="База" sheetId="3" r:id="rId2"/>
     <sheet name="Заявка" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -1280,8 +1280,8 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,9 +1592,9 @@
   </sheetPr>
   <dimension ref="A1:W601"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" zeroHeight="1" x14ac:dyDescent="0.4"/>
@@ -13717,7 +13717,7 @@
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>